<commit_message>
Change volume curve to square
</commit_message>
<xml_diff>
--- a/volumelog.xlsx
+++ b/volumelog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tim.SABRE\Documents\GitHub\UltranetReceiver\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC798934-4354-4AD1-9121-909524FA4E7B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FD70275-E5CC-4D49-9C76-B7466644F37C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="42120" yWindow="1470" windowWidth="33915" windowHeight="17385" xr2:uid="{2BD9426E-1403-469D-B89E-0B63E08128A8}"/>
   </bookViews>
@@ -149,385 +149,385 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>15</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>20</c:v>
+                  <c:v>100</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>25</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>30</c:v>
+                  <c:v>196</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35</c:v>
+                  <c:v>256</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>41</c:v>
+                  <c:v>324</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>47</c:v>
+                  <c:v>400</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>53</c:v>
+                  <c:v>484</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>60</c:v>
+                  <c:v>576</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>67</c:v>
+                  <c:v>676</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>74</c:v>
+                  <c:v>784</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>82</c:v>
+                  <c:v>900</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>90</c:v>
+                  <c:v>1024</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>99</c:v>
+                  <c:v>1156</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>108</c:v>
+                  <c:v>1296</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>118</c:v>
+                  <c:v>1444</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>129</c:v>
+                  <c:v>1600</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>139</c:v>
+                  <c:v>1764</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>151</c:v>
+                  <c:v>1936</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>163</c:v>
+                  <c:v>2116</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>176</c:v>
+                  <c:v>2304</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>189</c:v>
+                  <c:v>2500</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>204</c:v>
+                  <c:v>2704</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>219</c:v>
+                  <c:v>2916</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>235</c:v>
+                  <c:v>3136</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>251</c:v>
+                  <c:v>3364</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>269</c:v>
+                  <c:v>3600</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>288</c:v>
+                  <c:v>3844</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>308</c:v>
+                  <c:v>4096</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>328</c:v>
+                  <c:v>4356</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>351</c:v>
+                  <c:v>4624</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>374</c:v>
+                  <c:v>4900</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>398</c:v>
+                  <c:v>5184</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>424</c:v>
+                  <c:v>5476</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>452</c:v>
+                  <c:v>5776</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>481</c:v>
+                  <c:v>6084</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>511</c:v>
+                  <c:v>6400</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>544</c:v>
+                  <c:v>6724</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>578</c:v>
+                  <c:v>7056</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>614</c:v>
+                  <c:v>7396</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>652</c:v>
+                  <c:v>7744</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>692</c:v>
+                  <c:v>8100</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>734</c:v>
+                  <c:v>8464</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>779</c:v>
+                  <c:v>8836</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>826</c:v>
+                  <c:v>9216</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>876</c:v>
+                  <c:v>9604</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>929</c:v>
+                  <c:v>10000</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>984</c:v>
+                  <c:v>10404</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>1043</c:v>
+                  <c:v>10816</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1105</c:v>
+                  <c:v>11236</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1170</c:v>
+                  <c:v>11664</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1239</c:v>
+                  <c:v>12100</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>1312</c:v>
+                  <c:v>12544</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>1389</c:v>
+                  <c:v>12996</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1471</c:v>
+                  <c:v>13456</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>1557</c:v>
+                  <c:v>13924</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1647</c:v>
+                  <c:v>14400</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1743</c:v>
+                  <c:v>14884</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>1844</c:v>
+                  <c:v>15376</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>1951</c:v>
+                  <c:v>15876</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2064</c:v>
+                  <c:v>16384</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2183</c:v>
+                  <c:v>16900</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>2309</c:v>
+                  <c:v>17424</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2441</c:v>
+                  <c:v>17956</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>2581</c:v>
+                  <c:v>18496</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2729</c:v>
+                  <c:v>19044</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2886</c:v>
+                  <c:v>19600</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>3051</c:v>
+                  <c:v>20164</c:v>
                 </c:pt>
                 <c:pt idx="72">
-                  <c:v>3225</c:v>
+                  <c:v>20736</c:v>
                 </c:pt>
                 <c:pt idx="73">
-                  <c:v>3409</c:v>
+                  <c:v>21316</c:v>
                 </c:pt>
                 <c:pt idx="74">
-                  <c:v>3603</c:v>
+                  <c:v>21904</c:v>
                 </c:pt>
                 <c:pt idx="75">
-                  <c:v>3808</c:v>
+                  <c:v>22500</c:v>
                 </c:pt>
                 <c:pt idx="76">
-                  <c:v>4025</c:v>
+                  <c:v>23104</c:v>
                 </c:pt>
                 <c:pt idx="77">
-                  <c:v>4254</c:v>
+                  <c:v>23716</c:v>
                 </c:pt>
                 <c:pt idx="78">
-                  <c:v>4495</c:v>
+                  <c:v>24336</c:v>
                 </c:pt>
                 <c:pt idx="79">
-                  <c:v>4750</c:v>
+                  <c:v>24964</c:v>
                 </c:pt>
                 <c:pt idx="80">
-                  <c:v>5019</c:v>
+                  <c:v>25600</c:v>
                 </c:pt>
                 <c:pt idx="81">
-                  <c:v>5303</c:v>
+                  <c:v>26244</c:v>
                 </c:pt>
                 <c:pt idx="82">
-                  <c:v>5604</c:v>
+                  <c:v>26896</c:v>
                 </c:pt>
                 <c:pt idx="83">
-                  <c:v>5920</c:v>
+                  <c:v>27556</c:v>
                 </c:pt>
                 <c:pt idx="84">
-                  <c:v>6255</c:v>
+                  <c:v>28224</c:v>
                 </c:pt>
                 <c:pt idx="85">
-                  <c:v>6608</c:v>
+                  <c:v>28900</c:v>
                 </c:pt>
                 <c:pt idx="86">
-                  <c:v>6982</c:v>
+                  <c:v>29584</c:v>
                 </c:pt>
                 <c:pt idx="87">
-                  <c:v>7376</c:v>
+                  <c:v>30276</c:v>
                 </c:pt>
                 <c:pt idx="88">
-                  <c:v>7792</c:v>
+                  <c:v>30976</c:v>
                 </c:pt>
                 <c:pt idx="89">
-                  <c:v>8231</c:v>
+                  <c:v>31684</c:v>
                 </c:pt>
                 <c:pt idx="90">
-                  <c:v>8695</c:v>
+                  <c:v>32400</c:v>
                 </c:pt>
                 <c:pt idx="91">
-                  <c:v>9184</c:v>
+                  <c:v>33124</c:v>
                 </c:pt>
                 <c:pt idx="92">
-                  <c:v>9701</c:v>
+                  <c:v>33856</c:v>
                 </c:pt>
                 <c:pt idx="93">
-                  <c:v>10247</c:v>
+                  <c:v>34596</c:v>
                 </c:pt>
                 <c:pt idx="94">
-                  <c:v>10824</c:v>
+                  <c:v>35344</c:v>
                 </c:pt>
                 <c:pt idx="95">
-                  <c:v>11433</c:v>
+                  <c:v>36100</c:v>
                 </c:pt>
                 <c:pt idx="96">
-                  <c:v>12075</c:v>
+                  <c:v>36864</c:v>
                 </c:pt>
                 <c:pt idx="97">
-                  <c:v>12754</c:v>
+                  <c:v>37636</c:v>
                 </c:pt>
                 <c:pt idx="98">
-                  <c:v>13471</c:v>
+                  <c:v>38416</c:v>
                 </c:pt>
                 <c:pt idx="99">
-                  <c:v>14228</c:v>
+                  <c:v>39204</c:v>
                 </c:pt>
                 <c:pt idx="100">
-                  <c:v>15027</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
                 <c:pt idx="101">
-                  <c:v>15870</c:v>
+                  <c:v>40804</c:v>
                 </c:pt>
                 <c:pt idx="102">
-                  <c:v>16761</c:v>
+                  <c:v>41616</c:v>
                 </c:pt>
                 <c:pt idx="103">
-                  <c:v>17702</c:v>
+                  <c:v>42436</c:v>
                 </c:pt>
                 <c:pt idx="104">
-                  <c:v>18695</c:v>
+                  <c:v>43264</c:v>
                 </c:pt>
                 <c:pt idx="105">
-                  <c:v>19744</c:v>
+                  <c:v>44100</c:v>
                 </c:pt>
                 <c:pt idx="106">
-                  <c:v>20851</c:v>
+                  <c:v>44944</c:v>
                 </c:pt>
                 <c:pt idx="107">
-                  <c:v>22020</c:v>
+                  <c:v>45796</c:v>
                 </c:pt>
                 <c:pt idx="108">
-                  <c:v>23255</c:v>
+                  <c:v>46656</c:v>
                 </c:pt>
                 <c:pt idx="109">
-                  <c:v>24559</c:v>
+                  <c:v>47524</c:v>
                 </c:pt>
                 <c:pt idx="110">
-                  <c:v>25935</c:v>
+                  <c:v>48400</c:v>
                 </c:pt>
                 <c:pt idx="111">
-                  <c:v>27388</c:v>
+                  <c:v>49284</c:v>
                 </c:pt>
                 <c:pt idx="112">
-                  <c:v>28923</c:v>
+                  <c:v>50176</c:v>
                 </c:pt>
                 <c:pt idx="113">
-                  <c:v>30544</c:v>
+                  <c:v>51076</c:v>
                 </c:pt>
                 <c:pt idx="114">
-                  <c:v>32255</c:v>
+                  <c:v>51984</c:v>
                 </c:pt>
                 <c:pt idx="115">
-                  <c:v>34062</c:v>
+                  <c:v>52900</c:v>
                 </c:pt>
                 <c:pt idx="116">
-                  <c:v>35969</c:v>
+                  <c:v>53824</c:v>
                 </c:pt>
                 <c:pt idx="117">
-                  <c:v>37984</c:v>
+                  <c:v>54756</c:v>
                 </c:pt>
                 <c:pt idx="118">
-                  <c:v>40111</c:v>
+                  <c:v>55696</c:v>
                 </c:pt>
                 <c:pt idx="119">
-                  <c:v>42357</c:v>
+                  <c:v>56644</c:v>
                 </c:pt>
                 <c:pt idx="120">
-                  <c:v>44728</c:v>
+                  <c:v>57600</c:v>
                 </c:pt>
                 <c:pt idx="121">
-                  <c:v>47232</c:v>
+                  <c:v>58564</c:v>
                 </c:pt>
                 <c:pt idx="122">
-                  <c:v>49876</c:v>
+                  <c:v>59536</c:v>
                 </c:pt>
                 <c:pt idx="123">
-                  <c:v>52668</c:v>
+                  <c:v>60516</c:v>
                 </c:pt>
                 <c:pt idx="124">
-                  <c:v>55616</c:v>
+                  <c:v>61504</c:v>
                 </c:pt>
                 <c:pt idx="125">
-                  <c:v>58728</c:v>
+                  <c:v>62500</c:v>
                 </c:pt>
                 <c:pt idx="126">
-                  <c:v>62015</c:v>
+                  <c:v>63504</c:v>
                 </c:pt>
                 <c:pt idx="127">
-                  <c:v>65485</c:v>
+                  <c:v>64516</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1606,7 +1606,7 @@
   <dimension ref="A1:C128"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B1" sqref="B1:B128"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1615,9 +1615,9 @@
       <c r="A1">
         <v>0</v>
       </c>
-      <c r="B1" t="e">
-        <f>ROUND(65535*(1/(A1/127)+1)^2/1000,0)</f>
-        <v>#DIV/0!</v>
+      <c r="B1">
+        <f>ROUND(4*A1*A1,0)</f>
+        <v>0</v>
       </c>
       <c r="C1">
         <f>ROUND(65535*EXP(6.908*A1/127)/1000,0)-66</f>
@@ -1629,8 +1629,8 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <f t="shared" ref="B2:B65" si="0">ROUND(65535*EXP(6.908*A2/127)/1000,0)-66</f>
-        <v>3</v>
+        <f t="shared" ref="B2:B65" si="0">ROUND(4*A2*A2,0)</f>
+        <v>4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -1639,7 +1639,7 @@
       </c>
       <c r="B3">
         <f t="shared" si="0"/>
-        <v>7</v>
+        <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -1648,7 +1648,7 @@
       </c>
       <c r="B4">
         <f t="shared" si="0"/>
-        <v>11</v>
+        <v>36</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>15</v>
+        <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -1666,7 +1666,7 @@
       </c>
       <c r="B6">
         <f t="shared" si="0"/>
-        <v>20</v>
+        <v>100</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -1675,7 +1675,7 @@
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>25</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
@@ -1684,7 +1684,7 @@
       </c>
       <c r="B8">
         <f t="shared" si="0"/>
-        <v>30</v>
+        <v>196</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
@@ -1693,7 +1693,7 @@
       </c>
       <c r="B9">
         <f t="shared" si="0"/>
-        <v>35</v>
+        <v>256</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
@@ -1702,7 +1702,7 @@
       </c>
       <c r="B10">
         <f t="shared" si="0"/>
-        <v>41</v>
+        <v>324</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1711,7 +1711,7 @@
       </c>
       <c r="B11">
         <f t="shared" si="0"/>
-        <v>47</v>
+        <v>400</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
@@ -1720,7 +1720,7 @@
       </c>
       <c r="B12">
         <f t="shared" si="0"/>
-        <v>53</v>
+        <v>484</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
@@ -1729,7 +1729,7 @@
       </c>
       <c r="B13">
         <f t="shared" si="0"/>
-        <v>60</v>
+        <v>576</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
@@ -1738,7 +1738,7 @@
       </c>
       <c r="B14">
         <f t="shared" si="0"/>
-        <v>67</v>
+        <v>676</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
@@ -1747,7 +1747,7 @@
       </c>
       <c r="B15">
         <f t="shared" si="0"/>
-        <v>74</v>
+        <v>784</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
@@ -1756,7 +1756,7 @@
       </c>
       <c r="B16">
         <f t="shared" si="0"/>
-        <v>82</v>
+        <v>900</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
@@ -1765,7 +1765,7 @@
       </c>
       <c r="B17">
         <f t="shared" si="0"/>
-        <v>90</v>
+        <v>1024</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
@@ -1774,7 +1774,7 @@
       </c>
       <c r="B18">
         <f t="shared" si="0"/>
-        <v>99</v>
+        <v>1156</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
@@ -1783,7 +1783,7 @@
       </c>
       <c r="B19">
         <f t="shared" si="0"/>
-        <v>108</v>
+        <v>1296</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
@@ -1792,7 +1792,7 @@
       </c>
       <c r="B20">
         <f t="shared" si="0"/>
-        <v>118</v>
+        <v>1444</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
@@ -1801,7 +1801,7 @@
       </c>
       <c r="B21">
         <f t="shared" si="0"/>
-        <v>129</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
@@ -1810,7 +1810,7 @@
       </c>
       <c r="B22">
         <f t="shared" si="0"/>
-        <v>139</v>
+        <v>1764</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
@@ -1819,7 +1819,7 @@
       </c>
       <c r="B23">
         <f t="shared" si="0"/>
-        <v>151</v>
+        <v>1936</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
@@ -1828,7 +1828,7 @@
       </c>
       <c r="B24">
         <f t="shared" si="0"/>
-        <v>163</v>
+        <v>2116</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
@@ -1837,7 +1837,7 @@
       </c>
       <c r="B25">
         <f t="shared" si="0"/>
-        <v>176</v>
+        <v>2304</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
@@ -1846,7 +1846,7 @@
       </c>
       <c r="B26">
         <f t="shared" si="0"/>
-        <v>189</v>
+        <v>2500</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1855,7 +1855,7 @@
       </c>
       <c r="B27">
         <f t="shared" si="0"/>
-        <v>204</v>
+        <v>2704</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
@@ -1864,7 +1864,7 @@
       </c>
       <c r="B28">
         <f t="shared" si="0"/>
-        <v>219</v>
+        <v>2916</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
@@ -1873,7 +1873,7 @@
       </c>
       <c r="B29">
         <f t="shared" si="0"/>
-        <v>235</v>
+        <v>3136</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
@@ -1882,7 +1882,7 @@
       </c>
       <c r="B30">
         <f t="shared" si="0"/>
-        <v>251</v>
+        <v>3364</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1891,7 +1891,7 @@
       </c>
       <c r="B31">
         <f t="shared" si="0"/>
-        <v>269</v>
+        <v>3600</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
@@ -1900,7 +1900,7 @@
       </c>
       <c r="B32">
         <f t="shared" si="0"/>
-        <v>288</v>
+        <v>3844</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
@@ -1909,7 +1909,7 @@
       </c>
       <c r="B33">
         <f t="shared" si="0"/>
-        <v>308</v>
+        <v>4096</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1918,7 +1918,7 @@
       </c>
       <c r="B34">
         <f t="shared" si="0"/>
-        <v>328</v>
+        <v>4356</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -1927,7 +1927,7 @@
       </c>
       <c r="B35">
         <f t="shared" si="0"/>
-        <v>351</v>
+        <v>4624</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1936,7 +1936,7 @@
       </c>
       <c r="B36">
         <f t="shared" si="0"/>
-        <v>374</v>
+        <v>4900</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
@@ -1945,7 +1945,7 @@
       </c>
       <c r="B37">
         <f t="shared" si="0"/>
-        <v>398</v>
+        <v>5184</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
@@ -1954,7 +1954,7 @@
       </c>
       <c r="B38">
         <f t="shared" si="0"/>
-        <v>424</v>
+        <v>5476</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
@@ -1963,7 +1963,7 @@
       </c>
       <c r="B39">
         <f t="shared" si="0"/>
-        <v>452</v>
+        <v>5776</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
@@ -1972,7 +1972,7 @@
       </c>
       <c r="B40">
         <f t="shared" si="0"/>
-        <v>481</v>
+        <v>6084</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
@@ -1981,7 +1981,7 @@
       </c>
       <c r="B41">
         <f t="shared" si="0"/>
-        <v>511</v>
+        <v>6400</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
@@ -1990,7 +1990,7 @@
       </c>
       <c r="B42">
         <f t="shared" si="0"/>
-        <v>544</v>
+        <v>6724</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
@@ -1999,7 +1999,7 @@
       </c>
       <c r="B43">
         <f t="shared" si="0"/>
-        <v>578</v>
+        <v>7056</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
@@ -2008,7 +2008,7 @@
       </c>
       <c r="B44">
         <f t="shared" si="0"/>
-        <v>614</v>
+        <v>7396</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
@@ -2017,7 +2017,7 @@
       </c>
       <c r="B45">
         <f t="shared" si="0"/>
-        <v>652</v>
+        <v>7744</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -2026,7 +2026,7 @@
       </c>
       <c r="B46">
         <f t="shared" si="0"/>
-        <v>692</v>
+        <v>8100</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
@@ -2035,7 +2035,7 @@
       </c>
       <c r="B47">
         <f t="shared" si="0"/>
-        <v>734</v>
+        <v>8464</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -2044,7 +2044,7 @@
       </c>
       <c r="B48">
         <f t="shared" si="0"/>
-        <v>779</v>
+        <v>8836</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
@@ -2053,7 +2053,7 @@
       </c>
       <c r="B49">
         <f t="shared" si="0"/>
-        <v>826</v>
+        <v>9216</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
@@ -2062,7 +2062,7 @@
       </c>
       <c r="B50">
         <f t="shared" si="0"/>
-        <v>876</v>
+        <v>9604</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
@@ -2071,7 +2071,7 @@
       </c>
       <c r="B51">
         <f t="shared" si="0"/>
-        <v>929</v>
+        <v>10000</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
@@ -2080,7 +2080,7 @@
       </c>
       <c r="B52">
         <f t="shared" si="0"/>
-        <v>984</v>
+        <v>10404</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
@@ -2089,7 +2089,7 @@
       </c>
       <c r="B53">
         <f t="shared" si="0"/>
-        <v>1043</v>
+        <v>10816</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
@@ -2098,7 +2098,7 @@
       </c>
       <c r="B54">
         <f t="shared" si="0"/>
-        <v>1105</v>
+        <v>11236</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
@@ -2107,7 +2107,7 @@
       </c>
       <c r="B55">
         <f t="shared" si="0"/>
-        <v>1170</v>
+        <v>11664</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
@@ -2116,7 +2116,7 @@
       </c>
       <c r="B56">
         <f t="shared" si="0"/>
-        <v>1239</v>
+        <v>12100</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
@@ -2125,7 +2125,7 @@
       </c>
       <c r="B57">
         <f t="shared" si="0"/>
-        <v>1312</v>
+        <v>12544</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
@@ -2134,7 +2134,7 @@
       </c>
       <c r="B58">
         <f t="shared" si="0"/>
-        <v>1389</v>
+        <v>12996</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
@@ -2143,7 +2143,7 @@
       </c>
       <c r="B59">
         <f t="shared" si="0"/>
-        <v>1471</v>
+        <v>13456</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
@@ -2152,7 +2152,7 @@
       </c>
       <c r="B60">
         <f t="shared" si="0"/>
-        <v>1557</v>
+        <v>13924</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
@@ -2161,7 +2161,7 @@
       </c>
       <c r="B61">
         <f t="shared" si="0"/>
-        <v>1647</v>
+        <v>14400</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
@@ -2170,7 +2170,7 @@
       </c>
       <c r="B62">
         <f t="shared" si="0"/>
-        <v>1743</v>
+        <v>14884</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
@@ -2179,7 +2179,7 @@
       </c>
       <c r="B63">
         <f t="shared" si="0"/>
-        <v>1844</v>
+        <v>15376</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
@@ -2188,7 +2188,7 @@
       </c>
       <c r="B64">
         <f t="shared" si="0"/>
-        <v>1951</v>
+        <v>15876</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
@@ -2197,7 +2197,7 @@
       </c>
       <c r="B65">
         <f t="shared" si="0"/>
-        <v>2064</v>
+        <v>16384</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
@@ -2205,8 +2205,8 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <f t="shared" ref="B66:B128" si="1">ROUND(65535*EXP(6.908*A66/127)/1000,0)-66</f>
-        <v>2183</v>
+        <f t="shared" ref="B66:B128" si="1">ROUND(4*A66*A66,0)</f>
+        <v>16900</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
@@ -2215,7 +2215,7 @@
       </c>
       <c r="B67">
         <f t="shared" si="1"/>
-        <v>2309</v>
+        <v>17424</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
@@ -2224,7 +2224,7 @@
       </c>
       <c r="B68">
         <f t="shared" si="1"/>
-        <v>2441</v>
+        <v>17956</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
@@ -2233,7 +2233,7 @@
       </c>
       <c r="B69">
         <f t="shared" si="1"/>
-        <v>2581</v>
+        <v>18496</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
@@ -2242,7 +2242,7 @@
       </c>
       <c r="B70">
         <f t="shared" si="1"/>
-        <v>2729</v>
+        <v>19044</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
@@ -2251,7 +2251,7 @@
       </c>
       <c r="B71">
         <f t="shared" si="1"/>
-        <v>2886</v>
+        <v>19600</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
@@ -2260,7 +2260,7 @@
       </c>
       <c r="B72">
         <f t="shared" si="1"/>
-        <v>3051</v>
+        <v>20164</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
@@ -2269,7 +2269,7 @@
       </c>
       <c r="B73">
         <f t="shared" si="1"/>
-        <v>3225</v>
+        <v>20736</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
@@ -2278,7 +2278,7 @@
       </c>
       <c r="B74">
         <f t="shared" si="1"/>
-        <v>3409</v>
+        <v>21316</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
@@ -2287,7 +2287,7 @@
       </c>
       <c r="B75">
         <f t="shared" si="1"/>
-        <v>3603</v>
+        <v>21904</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
@@ -2296,7 +2296,7 @@
       </c>
       <c r="B76">
         <f t="shared" si="1"/>
-        <v>3808</v>
+        <v>22500</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
@@ -2305,7 +2305,7 @@
       </c>
       <c r="B77">
         <f t="shared" si="1"/>
-        <v>4025</v>
+        <v>23104</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
@@ -2314,7 +2314,7 @@
       </c>
       <c r="B78">
         <f t="shared" si="1"/>
-        <v>4254</v>
+        <v>23716</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
@@ -2323,7 +2323,7 @@
       </c>
       <c r="B79">
         <f t="shared" si="1"/>
-        <v>4495</v>
+        <v>24336</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
@@ -2332,7 +2332,7 @@
       </c>
       <c r="B80">
         <f t="shared" si="1"/>
-        <v>4750</v>
+        <v>24964</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
@@ -2341,7 +2341,7 @@
       </c>
       <c r="B81">
         <f t="shared" si="1"/>
-        <v>5019</v>
+        <v>25600</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
@@ -2350,7 +2350,7 @@
       </c>
       <c r="B82">
         <f t="shared" si="1"/>
-        <v>5303</v>
+        <v>26244</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
@@ -2359,7 +2359,7 @@
       </c>
       <c r="B83">
         <f t="shared" si="1"/>
-        <v>5604</v>
+        <v>26896</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
@@ -2368,7 +2368,7 @@
       </c>
       <c r="B84">
         <f t="shared" si="1"/>
-        <v>5920</v>
+        <v>27556</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
@@ -2377,7 +2377,7 @@
       </c>
       <c r="B85">
         <f t="shared" si="1"/>
-        <v>6255</v>
+        <v>28224</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
@@ -2386,7 +2386,7 @@
       </c>
       <c r="B86">
         <f t="shared" si="1"/>
-        <v>6608</v>
+        <v>28900</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
@@ -2395,7 +2395,7 @@
       </c>
       <c r="B87">
         <f t="shared" si="1"/>
-        <v>6982</v>
+        <v>29584</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
@@ -2404,7 +2404,7 @@
       </c>
       <c r="B88">
         <f t="shared" si="1"/>
-        <v>7376</v>
+        <v>30276</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
@@ -2413,7 +2413,7 @@
       </c>
       <c r="B89">
         <f t="shared" si="1"/>
-        <v>7792</v>
+        <v>30976</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
@@ -2422,7 +2422,7 @@
       </c>
       <c r="B90">
         <f t="shared" si="1"/>
-        <v>8231</v>
+        <v>31684</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
@@ -2431,7 +2431,7 @@
       </c>
       <c r="B91">
         <f t="shared" si="1"/>
-        <v>8695</v>
+        <v>32400</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
@@ -2440,7 +2440,7 @@
       </c>
       <c r="B92">
         <f t="shared" si="1"/>
-        <v>9184</v>
+        <v>33124</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
@@ -2449,7 +2449,7 @@
       </c>
       <c r="B93">
         <f t="shared" si="1"/>
-        <v>9701</v>
+        <v>33856</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
@@ -2458,7 +2458,7 @@
       </c>
       <c r="B94">
         <f t="shared" si="1"/>
-        <v>10247</v>
+        <v>34596</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
@@ -2467,7 +2467,7 @@
       </c>
       <c r="B95">
         <f t="shared" si="1"/>
-        <v>10824</v>
+        <v>35344</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
@@ -2476,7 +2476,7 @@
       </c>
       <c r="B96">
         <f t="shared" si="1"/>
-        <v>11433</v>
+        <v>36100</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
@@ -2485,7 +2485,7 @@
       </c>
       <c r="B97">
         <f t="shared" si="1"/>
-        <v>12075</v>
+        <v>36864</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
@@ -2494,7 +2494,7 @@
       </c>
       <c r="B98">
         <f t="shared" si="1"/>
-        <v>12754</v>
+        <v>37636</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
@@ -2503,7 +2503,7 @@
       </c>
       <c r="B99">
         <f t="shared" si="1"/>
-        <v>13471</v>
+        <v>38416</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
@@ -2512,7 +2512,7 @@
       </c>
       <c r="B100">
         <f t="shared" si="1"/>
-        <v>14228</v>
+        <v>39204</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
@@ -2521,7 +2521,7 @@
       </c>
       <c r="B101">
         <f t="shared" si="1"/>
-        <v>15027</v>
+        <v>40000</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
@@ -2530,7 +2530,7 @@
       </c>
       <c r="B102">
         <f t="shared" si="1"/>
-        <v>15870</v>
+        <v>40804</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
@@ -2539,7 +2539,7 @@
       </c>
       <c r="B103">
         <f t="shared" si="1"/>
-        <v>16761</v>
+        <v>41616</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
@@ -2548,7 +2548,7 @@
       </c>
       <c r="B104">
         <f t="shared" si="1"/>
-        <v>17702</v>
+        <v>42436</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
@@ -2557,7 +2557,7 @@
       </c>
       <c r="B105">
         <f t="shared" si="1"/>
-        <v>18695</v>
+        <v>43264</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
@@ -2566,7 +2566,7 @@
       </c>
       <c r="B106">
         <f t="shared" si="1"/>
-        <v>19744</v>
+        <v>44100</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
@@ -2575,7 +2575,7 @@
       </c>
       <c r="B107">
         <f t="shared" si="1"/>
-        <v>20851</v>
+        <v>44944</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
@@ -2584,7 +2584,7 @@
       </c>
       <c r="B108">
         <f t="shared" si="1"/>
-        <v>22020</v>
+        <v>45796</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
@@ -2593,7 +2593,7 @@
       </c>
       <c r="B109">
         <f t="shared" si="1"/>
-        <v>23255</v>
+        <v>46656</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
@@ -2602,7 +2602,7 @@
       </c>
       <c r="B110">
         <f t="shared" si="1"/>
-        <v>24559</v>
+        <v>47524</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
@@ -2611,7 +2611,7 @@
       </c>
       <c r="B111">
         <f t="shared" si="1"/>
-        <v>25935</v>
+        <v>48400</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
@@ -2620,7 +2620,7 @@
       </c>
       <c r="B112">
         <f t="shared" si="1"/>
-        <v>27388</v>
+        <v>49284</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
@@ -2629,7 +2629,7 @@
       </c>
       <c r="B113">
         <f t="shared" si="1"/>
-        <v>28923</v>
+        <v>50176</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
@@ -2638,7 +2638,7 @@
       </c>
       <c r="B114">
         <f t="shared" si="1"/>
-        <v>30544</v>
+        <v>51076</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
@@ -2647,7 +2647,7 @@
       </c>
       <c r="B115">
         <f t="shared" si="1"/>
-        <v>32255</v>
+        <v>51984</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
@@ -2656,7 +2656,7 @@
       </c>
       <c r="B116">
         <f t="shared" si="1"/>
-        <v>34062</v>
+        <v>52900</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
@@ -2665,7 +2665,7 @@
       </c>
       <c r="B117">
         <f t="shared" si="1"/>
-        <v>35969</v>
+        <v>53824</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
@@ -2674,7 +2674,7 @@
       </c>
       <c r="B118">
         <f t="shared" si="1"/>
-        <v>37984</v>
+        <v>54756</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
@@ -2683,7 +2683,7 @@
       </c>
       <c r="B119">
         <f t="shared" si="1"/>
-        <v>40111</v>
+        <v>55696</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
@@ -2692,7 +2692,7 @@
       </c>
       <c r="B120">
         <f t="shared" si="1"/>
-        <v>42357</v>
+        <v>56644</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
@@ -2701,7 +2701,7 @@
       </c>
       <c r="B121">
         <f t="shared" si="1"/>
-        <v>44728</v>
+        <v>57600</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
@@ -2710,7 +2710,7 @@
       </c>
       <c r="B122">
         <f t="shared" si="1"/>
-        <v>47232</v>
+        <v>58564</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
@@ -2719,7 +2719,7 @@
       </c>
       <c r="B123">
         <f t="shared" si="1"/>
-        <v>49876</v>
+        <v>59536</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
@@ -2728,7 +2728,7 @@
       </c>
       <c r="B124">
         <f t="shared" si="1"/>
-        <v>52668</v>
+        <v>60516</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
@@ -2737,7 +2737,7 @@
       </c>
       <c r="B125">
         <f t="shared" si="1"/>
-        <v>55616</v>
+        <v>61504</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
@@ -2746,7 +2746,7 @@
       </c>
       <c r="B126">
         <f t="shared" si="1"/>
-        <v>58728</v>
+        <v>62500</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
@@ -2755,7 +2755,7 @@
       </c>
       <c r="B127">
         <f t="shared" si="1"/>
-        <v>62015</v>
+        <v>63504</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
@@ -2764,7 +2764,7 @@
       </c>
       <c r="B128">
         <f t="shared" si="1"/>
-        <v>65485</v>
+        <v>64516</v>
       </c>
     </row>
   </sheetData>

</xml_diff>